<commit_message>
tested on test dataset and generated test_result
</commit_message>
<xml_diff>
--- a/test_result.xlsx
+++ b/test_result.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24729"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mufad\python_mlprojects\arduino-signal\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{505B393C-0579-4AE8-A0EC-A03CCA00BE7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -37,8 +31,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -101,14 +95,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -155,7 +141,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -187,27 +173,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -239,24 +207,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -432,1748 +382,2115 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D124"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E124"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
+    <row r="1" spans="1:5">
       <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2">
+    <row r="2" spans="1:5">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2">
         <v>1702</v>
       </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
       <c r="C2">
         <v>0</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3">
         <v>3412</v>
       </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4">
+      <c r="E3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4">
         <v>5116</v>
       </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
       <c r="C4">
         <v>0</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5">
+      <c r="E4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5">
         <v>6828</v>
       </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
       <c r="C5">
         <v>0</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6">
+      <c r="E5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6">
         <v>8535</v>
       </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
       <c r="C6">
         <v>0</v>
       </c>
       <c r="D6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7">
+      <c r="E6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7">
         <v>8532</v>
       </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
       <c r="C7">
         <v>0</v>
       </c>
       <c r="D7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8">
+      <c r="E7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8">
         <v>8543</v>
       </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
       <c r="C8">
         <v>0</v>
       </c>
       <c r="D8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9">
+      <c r="E8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9">
         <v>8538</v>
       </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
       <c r="C9">
         <v>0</v>
       </c>
       <c r="D9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10">
+      <c r="E9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10">
         <v>8518</v>
       </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
       <c r="C10">
         <v>0</v>
       </c>
       <c r="D10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11">
+      <c r="E10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11">
         <v>8496</v>
       </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
       <c r="C11">
         <v>0</v>
       </c>
       <c r="D11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12">
+      <c r="E11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12">
         <v>8481</v>
       </c>
-      <c r="B12">
-        <v>0</v>
-      </c>
       <c r="C12">
         <v>0</v>
       </c>
       <c r="D12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13">
+      <c r="E12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13">
         <v>8456</v>
       </c>
-      <c r="B13">
-        <v>0</v>
-      </c>
       <c r="C13">
         <v>0</v>
       </c>
       <c r="D13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14">
+      <c r="E13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14">
         <v>8453</v>
       </c>
-      <c r="B14">
-        <v>0</v>
-      </c>
       <c r="C14">
         <v>0</v>
       </c>
       <c r="D14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15">
+      <c r="E14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15">
         <v>8457</v>
       </c>
-      <c r="B15">
-        <v>0</v>
-      </c>
       <c r="C15">
         <v>0</v>
       </c>
       <c r="D15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16">
+      <c r="E15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16">
         <v>8488</v>
       </c>
-      <c r="B16">
-        <v>0</v>
-      </c>
       <c r="C16">
         <v>0</v>
       </c>
       <c r="D16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17">
+      <c r="E16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17">
         <v>8512</v>
       </c>
-      <c r="B17">
-        <v>0</v>
-      </c>
       <c r="C17">
         <v>0</v>
       </c>
       <c r="D17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18">
+      <c r="E17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18">
         <v>8515</v>
       </c>
-      <c r="B18">
-        <v>0</v>
-      </c>
       <c r="C18">
         <v>0</v>
       </c>
       <c r="D18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19">
+      <c r="E18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19">
         <v>8542</v>
       </c>
-      <c r="B19">
-        <v>0</v>
-      </c>
       <c r="C19">
         <v>0</v>
       </c>
       <c r="D19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20">
+      <c r="E19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20">
         <v>8542</v>
       </c>
-      <c r="B20">
-        <v>0</v>
-      </c>
       <c r="C20">
         <v>0</v>
       </c>
       <c r="D20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21">
+      <c r="E20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="B21">
         <v>8512</v>
       </c>
-      <c r="B21">
-        <v>0</v>
-      </c>
       <c r="C21">
         <v>0</v>
       </c>
       <c r="D21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22">
+      <c r="E21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="B22">
         <v>8498</v>
       </c>
-      <c r="B22">
-        <v>0</v>
-      </c>
       <c r="C22">
         <v>0</v>
       </c>
       <c r="D22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23">
+      <c r="E22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="1">
+        <v>21</v>
+      </c>
+      <c r="B23">
         <v>8505</v>
       </c>
-      <c r="B23">
-        <v>0</v>
-      </c>
       <c r="C23">
         <v>0</v>
       </c>
       <c r="D23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24">
+      <c r="E23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="1">
+        <v>22</v>
+      </c>
+      <c r="B24">
         <v>8454</v>
       </c>
-      <c r="B24">
-        <v>0</v>
-      </c>
       <c r="C24">
         <v>0</v>
       </c>
       <c r="D24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25">
+      <c r="E24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="1">
+        <v>23</v>
+      </c>
+      <c r="B25">
         <v>8469</v>
       </c>
-      <c r="B25">
-        <v>0</v>
-      </c>
       <c r="C25">
         <v>0</v>
       </c>
       <c r="D25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26">
+      <c r="E25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="1">
+        <v>24</v>
+      </c>
+      <c r="B26">
         <v>8476</v>
       </c>
-      <c r="B26">
-        <v>0</v>
-      </c>
       <c r="C26">
         <v>0</v>
       </c>
       <c r="D26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27">
+      <c r="E26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="1">
+        <v>25</v>
+      </c>
+      <c r="B27">
         <v>8498</v>
       </c>
-      <c r="B27">
-        <v>0</v>
-      </c>
       <c r="C27">
         <v>0</v>
       </c>
       <c r="D27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28">
+      <c r="E27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="1">
+        <v>26</v>
+      </c>
+      <c r="B28">
         <v>8488</v>
       </c>
-      <c r="B28">
-        <v>0</v>
-      </c>
       <c r="C28">
         <v>0</v>
       </c>
       <c r="D28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29">
+      <c r="E28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="1">
+        <v>27</v>
+      </c>
+      <c r="B29">
         <v>8525</v>
       </c>
-      <c r="B29">
-        <v>0</v>
-      </c>
       <c r="C29">
         <v>0</v>
       </c>
       <c r="D29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30">
+      <c r="E29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="1">
+        <v>28</v>
+      </c>
+      <c r="B30">
         <v>8500</v>
       </c>
-      <c r="B30">
-        <v>0</v>
-      </c>
       <c r="C30">
         <v>0</v>
       </c>
       <c r="D30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31">
+      <c r="E30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="1">
+        <v>29</v>
+      </c>
+      <c r="B31">
         <v>8496</v>
       </c>
-      <c r="B31">
-        <v>0</v>
-      </c>
       <c r="C31">
         <v>0</v>
       </c>
       <c r="D31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32">
+      <c r="E31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="1">
+        <v>30</v>
+      </c>
+      <c r="B32">
         <v>8486</v>
       </c>
-      <c r="B32">
-        <v>0</v>
-      </c>
       <c r="C32">
         <v>0</v>
       </c>
       <c r="D32">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33">
+      <c r="E32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="1">
+        <v>31</v>
+      </c>
+      <c r="B33">
         <v>8510</v>
       </c>
-      <c r="B33">
-        <v>0</v>
-      </c>
       <c r="C33">
         <v>0</v>
       </c>
       <c r="D33">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34">
+      <c r="E33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="1">
+        <v>32</v>
+      </c>
+      <c r="B34">
         <v>8505</v>
       </c>
-      <c r="B34">
-        <v>0</v>
-      </c>
       <c r="C34">
         <v>0</v>
       </c>
       <c r="D34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35">
+      <c r="E34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="1">
+        <v>33</v>
+      </c>
+      <c r="B35">
         <v>8504</v>
       </c>
-      <c r="B35">
-        <v>0</v>
-      </c>
       <c r="C35">
         <v>0</v>
       </c>
       <c r="D35">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36">
+      <c r="E35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="1">
+        <v>34</v>
+      </c>
+      <c r="B36">
         <v>8523</v>
       </c>
-      <c r="B36">
-        <v>0</v>
-      </c>
       <c r="C36">
         <v>0</v>
       </c>
       <c r="D36">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37">
+      <c r="E36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="1">
+        <v>35</v>
+      </c>
+      <c r="B37">
         <v>8513</v>
       </c>
-      <c r="B37">
-        <v>0</v>
-      </c>
       <c r="C37">
         <v>0</v>
       </c>
       <c r="D37">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38">
+      <c r="E37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="1">
+        <v>36</v>
+      </c>
+      <c r="B38">
         <v>8497</v>
       </c>
-      <c r="B38">
-        <v>0</v>
-      </c>
       <c r="C38">
         <v>0</v>
       </c>
       <c r="D38">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39">
+      <c r="E38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="1">
+        <v>37</v>
+      </c>
+      <c r="B39">
         <v>8484</v>
       </c>
-      <c r="B39">
-        <v>0</v>
-      </c>
       <c r="C39">
         <v>0</v>
       </c>
       <c r="D39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40">
+      <c r="E39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="1">
+        <v>38</v>
+      </c>
+      <c r="B40">
         <v>8479</v>
       </c>
-      <c r="B40">
-        <v>0</v>
-      </c>
       <c r="C40">
         <v>0</v>
       </c>
       <c r="D40">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41">
+      <c r="E40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="1">
+        <v>39</v>
+      </c>
+      <c r="B41">
         <v>8468</v>
       </c>
-      <c r="B41">
-        <v>0</v>
-      </c>
       <c r="C41">
         <v>0</v>
       </c>
       <c r="D41">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42">
+      <c r="E41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="1">
+        <v>40</v>
+      </c>
+      <c r="B42">
         <v>8465</v>
       </c>
-      <c r="B42">
-        <v>0</v>
-      </c>
       <c r="C42">
         <v>0</v>
       </c>
       <c r="D42">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43">
+      <c r="E42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="1">
+        <v>41</v>
+      </c>
+      <c r="B43">
         <v>8444</v>
       </c>
-      <c r="B43">
-        <v>0</v>
-      </c>
       <c r="C43">
         <v>0</v>
       </c>
       <c r="D43">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44">
+      <c r="E43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" s="1">
+        <v>42</v>
+      </c>
+      <c r="B44">
         <v>8461</v>
       </c>
-      <c r="B44">
-        <v>0</v>
-      </c>
       <c r="C44">
         <v>0</v>
       </c>
       <c r="D44">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45">
+      <c r="E44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" s="1">
+        <v>43</v>
+      </c>
+      <c r="B45">
         <v>8473</v>
       </c>
-      <c r="B45">
-        <v>0</v>
-      </c>
       <c r="C45">
         <v>0</v>
       </c>
       <c r="D45">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46">
+      <c r="E45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" s="1">
+        <v>44</v>
+      </c>
+      <c r="B46">
         <v>8478</v>
       </c>
-      <c r="B46">
-        <v>0</v>
-      </c>
       <c r="C46">
         <v>0</v>
       </c>
       <c r="D46">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47">
+      <c r="E46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" s="1">
+        <v>45</v>
+      </c>
+      <c r="B47">
         <v>8484</v>
       </c>
-      <c r="B47">
-        <v>0</v>
-      </c>
       <c r="C47">
         <v>0</v>
       </c>
       <c r="D47">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48">
+      <c r="E47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" s="1">
+        <v>46</v>
+      </c>
+      <c r="B48">
         <v>8485</v>
       </c>
-      <c r="B48">
-        <v>0</v>
-      </c>
       <c r="C48">
         <v>0</v>
       </c>
       <c r="D48">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49">
+      <c r="E48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" s="1">
+        <v>47</v>
+      </c>
+      <c r="B49">
         <v>8485</v>
       </c>
-      <c r="B49">
-        <v>0</v>
-      </c>
       <c r="C49">
         <v>0</v>
       </c>
       <c r="D49">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50">
+      <c r="E49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" s="1">
+        <v>48</v>
+      </c>
+      <c r="B50">
         <v>8492</v>
       </c>
-      <c r="B50">
-        <v>0</v>
-      </c>
       <c r="C50">
         <v>0</v>
       </c>
       <c r="D50">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A51">
+      <c r="E50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" s="1">
+        <v>49</v>
+      </c>
+      <c r="B51">
         <v>8483</v>
       </c>
-      <c r="B51">
-        <v>0</v>
-      </c>
       <c r="C51">
         <v>0</v>
       </c>
       <c r="D51">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52">
+      <c r="E51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" s="1">
+        <v>50</v>
+      </c>
+      <c r="B52">
         <v>8481</v>
       </c>
-      <c r="B52">
-        <v>0</v>
-      </c>
       <c r="C52">
         <v>0</v>
       </c>
       <c r="D52">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53">
+      <c r="E52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" s="1">
+        <v>51</v>
+      </c>
+      <c r="B53">
         <v>8498</v>
       </c>
-      <c r="B53">
-        <v>0</v>
-      </c>
       <c r="C53">
         <v>0</v>
       </c>
       <c r="D53">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54">
+      <c r="E53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" s="1">
+        <v>52</v>
+      </c>
+      <c r="B54">
         <v>8494</v>
       </c>
-      <c r="B54">
-        <v>0</v>
-      </c>
       <c r="C54">
         <v>0</v>
       </c>
       <c r="D54">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A55">
+      <c r="E54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" s="1">
+        <v>53</v>
+      </c>
+      <c r="B55">
         <v>8476</v>
       </c>
-      <c r="B55">
-        <v>0</v>
-      </c>
       <c r="C55">
         <v>0</v>
       </c>
       <c r="D55">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A56">
+      <c r="E55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" s="1">
+        <v>54</v>
+      </c>
+      <c r="B56">
         <v>8516</v>
       </c>
-      <c r="B56">
-        <v>0</v>
-      </c>
       <c r="C56">
         <v>0</v>
       </c>
       <c r="D56">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57">
+      <c r="E56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" s="1">
+        <v>55</v>
+      </c>
+      <c r="B57">
         <v>8513</v>
       </c>
-      <c r="B57">
-        <v>0</v>
-      </c>
       <c r="C57">
         <v>0</v>
       </c>
       <c r="D57">
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58">
+      <c r="E57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" s="1">
+        <v>56</v>
+      </c>
+      <c r="B58">
         <v>8524</v>
       </c>
-      <c r="B58">
-        <v>0</v>
-      </c>
       <c r="C58">
         <v>0</v>
       </c>
       <c r="D58">
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A59">
+      <c r="E58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" s="1">
+        <v>57</v>
+      </c>
+      <c r="B59">
         <v>8495</v>
       </c>
-      <c r="B59">
-        <v>0</v>
-      </c>
       <c r="C59">
         <v>0</v>
       </c>
       <c r="D59">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A60">
+      <c r="E59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" s="1">
+        <v>58</v>
+      </c>
+      <c r="B60">
         <v>8499</v>
       </c>
-      <c r="B60">
-        <v>0</v>
-      </c>
       <c r="C60">
         <v>0</v>
       </c>
       <c r="D60">
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A61">
+      <c r="E60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" s="1">
+        <v>59</v>
+      </c>
+      <c r="B61">
         <v>8486</v>
       </c>
-      <c r="B61">
-        <v>0</v>
-      </c>
       <c r="C61">
         <v>0</v>
       </c>
       <c r="D61">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A62">
+      <c r="E61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" s="1">
+        <v>60</v>
+      </c>
+      <c r="B62">
         <v>8484</v>
       </c>
-      <c r="B62">
-        <v>0</v>
-      </c>
       <c r="C62">
         <v>0</v>
       </c>
       <c r="D62">
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A63">
+      <c r="E62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" s="1">
+        <v>61</v>
+      </c>
+      <c r="B63">
         <v>8471</v>
       </c>
-      <c r="B63">
-        <v>0</v>
-      </c>
       <c r="C63">
         <v>0</v>
       </c>
       <c r="D63">
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A64">
+      <c r="E63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" s="1">
+        <v>62</v>
+      </c>
+      <c r="B64">
         <v>8493</v>
       </c>
-      <c r="B64">
-        <v>0</v>
-      </c>
       <c r="C64">
         <v>0</v>
       </c>
       <c r="D64">
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A65">
+      <c r="E64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" s="1">
+        <v>63</v>
+      </c>
+      <c r="B65">
         <v>8501</v>
       </c>
-      <c r="B65">
-        <v>0</v>
-      </c>
       <c r="C65">
         <v>0</v>
       </c>
       <c r="D65">
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A66">
+      <c r="E65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66" s="1">
+        <v>64</v>
+      </c>
+      <c r="B66">
         <v>8479</v>
       </c>
-      <c r="B66">
-        <v>0</v>
-      </c>
       <c r="C66">
         <v>0</v>
       </c>
       <c r="D66">
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A67">
+      <c r="E66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" s="1">
+        <v>65</v>
+      </c>
+      <c r="B67">
         <v>8475</v>
       </c>
-      <c r="B67">
-        <v>0</v>
-      </c>
       <c r="C67">
         <v>0</v>
       </c>
       <c r="D67">
         <v>0</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68">
+      <c r="E67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68" s="1">
+        <v>66</v>
+      </c>
+      <c r="B68">
         <v>8477</v>
       </c>
-      <c r="B68">
-        <v>0</v>
-      </c>
       <c r="C68">
         <v>0</v>
       </c>
       <c r="D68">
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A69">
+      <c r="E68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69" s="1">
+        <v>67</v>
+      </c>
+      <c r="B69">
         <v>8485</v>
       </c>
-      <c r="B69">
-        <v>0</v>
-      </c>
       <c r="C69">
         <v>0</v>
       </c>
       <c r="D69">
         <v>0</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A70">
+      <c r="E69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70" s="1">
+        <v>68</v>
+      </c>
+      <c r="B70">
         <v>8488</v>
       </c>
-      <c r="B70">
-        <v>0</v>
-      </c>
       <c r="C70">
         <v>0</v>
       </c>
       <c r="D70">
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A71">
+      <c r="E70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71" s="1">
+        <v>69</v>
+      </c>
+      <c r="B71">
         <v>8497</v>
       </c>
-      <c r="B71">
-        <v>0</v>
-      </c>
       <c r="C71">
         <v>0</v>
       </c>
       <c r="D71">
         <v>0</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A72">
+      <c r="E71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72" s="1">
+        <v>70</v>
+      </c>
+      <c r="B72">
         <v>8512</v>
       </c>
-      <c r="B72">
-        <v>0</v>
-      </c>
       <c r="C72">
         <v>0</v>
       </c>
       <c r="D72">
         <v>0</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A73">
+      <c r="E72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73" s="1">
+        <v>71</v>
+      </c>
+      <c r="B73">
         <v>8513</v>
       </c>
-      <c r="B73">
-        <v>0</v>
-      </c>
       <c r="C73">
         <v>0</v>
       </c>
       <c r="D73">
         <v>0</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A74">
+      <c r="E73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74" s="1">
+        <v>72</v>
+      </c>
+      <c r="B74">
         <v>8519</v>
       </c>
-      <c r="B74">
-        <v>0</v>
-      </c>
       <c r="C74">
         <v>0</v>
       </c>
       <c r="D74">
         <v>0</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A75">
+      <c r="E74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75" s="1">
+        <v>73</v>
+      </c>
+      <c r="B75">
         <v>8516</v>
       </c>
-      <c r="B75">
-        <v>0</v>
-      </c>
       <c r="C75">
         <v>0</v>
       </c>
       <c r="D75">
         <v>0</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A76">
+      <c r="E75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76" s="1">
+        <v>74</v>
+      </c>
+      <c r="B76">
         <v>8488</v>
       </c>
-      <c r="B76">
-        <v>0</v>
-      </c>
       <c r="C76">
         <v>0</v>
       </c>
       <c r="D76">
         <v>0</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A77">
+      <c r="E76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77" s="1">
+        <v>75</v>
+      </c>
+      <c r="B77">
         <v>8471</v>
       </c>
-      <c r="B77">
-        <v>0</v>
-      </c>
       <c r="C77">
         <v>0</v>
       </c>
       <c r="D77">
         <v>0</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A78">
+      <c r="E77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
+      <c r="A78" s="1">
+        <v>76</v>
+      </c>
+      <c r="B78">
         <v>8457</v>
       </c>
-      <c r="B78">
-        <v>0</v>
-      </c>
       <c r="C78">
         <v>0</v>
       </c>
       <c r="D78">
         <v>0</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A79">
+      <c r="E78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
+      <c r="A79" s="1">
+        <v>77</v>
+      </c>
+      <c r="B79">
         <v>8442</v>
       </c>
-      <c r="B79">
-        <v>0</v>
-      </c>
       <c r="C79">
         <v>0</v>
       </c>
       <c r="D79">
         <v>0</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A80">
+      <c r="E79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
+      <c r="A80" s="1">
+        <v>78</v>
+      </c>
+      <c r="B80">
         <v>8452</v>
       </c>
-      <c r="B80">
-        <v>0</v>
-      </c>
       <c r="C80">
         <v>0</v>
       </c>
       <c r="D80">
         <v>0</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A81">
+      <c r="E80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
+      <c r="A81" s="1">
+        <v>79</v>
+      </c>
+      <c r="B81">
         <v>8456</v>
       </c>
-      <c r="B81">
-        <v>0</v>
-      </c>
       <c r="C81">
         <v>0</v>
       </c>
       <c r="D81">
         <v>0</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A82">
+      <c r="E81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
+      <c r="A82" s="1">
+        <v>80</v>
+      </c>
+      <c r="B82">
         <v>8463</v>
       </c>
-      <c r="B82">
-        <v>0</v>
-      </c>
       <c r="C82">
         <v>0</v>
       </c>
       <c r="D82">
         <v>0</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A83">
+      <c r="E82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5">
+      <c r="A83" s="1">
+        <v>81</v>
+      </c>
+      <c r="B83">
         <v>8480</v>
       </c>
-      <c r="B83">
-        <v>0</v>
-      </c>
       <c r="C83">
         <v>0</v>
       </c>
       <c r="D83">
         <v>0</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A84">
+      <c r="E83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5">
+      <c r="A84" s="1">
+        <v>82</v>
+      </c>
+      <c r="B84">
         <v>8484</v>
       </c>
-      <c r="B84">
-        <v>0</v>
-      </c>
       <c r="C84">
         <v>0</v>
       </c>
       <c r="D84">
         <v>0</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A85">
+      <c r="E84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5">
+      <c r="A85" s="1">
+        <v>83</v>
+      </c>
+      <c r="B85">
         <v>8475</v>
       </c>
-      <c r="B85">
-        <v>0</v>
-      </c>
       <c r="C85">
         <v>0</v>
       </c>
       <c r="D85">
         <v>0</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A86">
+      <c r="E85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
+      <c r="A86" s="1">
+        <v>84</v>
+      </c>
+      <c r="B86">
         <v>8501</v>
       </c>
-      <c r="B86">
-        <v>0</v>
-      </c>
       <c r="C86">
         <v>0</v>
       </c>
       <c r="D86">
         <v>0</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A87">
+      <c r="E86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5">
+      <c r="A87" s="1">
+        <v>85</v>
+      </c>
+      <c r="B87">
         <v>8518</v>
       </c>
-      <c r="B87">
-        <v>0</v>
-      </c>
       <c r="C87">
         <v>0</v>
       </c>
       <c r="D87">
         <v>0</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A88">
+      <c r="E87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5">
+      <c r="A88" s="1">
+        <v>86</v>
+      </c>
+      <c r="B88">
         <v>8514</v>
       </c>
-      <c r="B88">
-        <v>0</v>
-      </c>
       <c r="C88">
         <v>0</v>
       </c>
       <c r="D88">
         <v>0</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A89">
+      <c r="E88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5">
+      <c r="A89" s="1">
+        <v>87</v>
+      </c>
+      <c r="B89">
         <v>8488</v>
       </c>
-      <c r="B89">
-        <v>0</v>
-      </c>
       <c r="C89">
         <v>0</v>
       </c>
       <c r="D89">
         <v>0</v>
       </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A90">
+      <c r="E89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
+      <c r="A90" s="1">
+        <v>88</v>
+      </c>
+      <c r="B90">
         <v>8501</v>
       </c>
-      <c r="B90">
-        <v>0</v>
-      </c>
       <c r="C90">
         <v>0</v>
       </c>
       <c r="D90">
         <v>0</v>
       </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A91">
+      <c r="E90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5">
+      <c r="A91" s="1">
+        <v>89</v>
+      </c>
+      <c r="B91">
         <v>8508</v>
       </c>
-      <c r="B91">
-        <v>0</v>
-      </c>
       <c r="C91">
         <v>0</v>
       </c>
       <c r="D91">
         <v>0</v>
       </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A92">
+      <c r="E91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5">
+      <c r="A92" s="1">
+        <v>90</v>
+      </c>
+      <c r="B92">
         <v>8500</v>
       </c>
-      <c r="B92">
-        <v>0</v>
-      </c>
       <c r="C92">
         <v>0</v>
       </c>
       <c r="D92">
         <v>0</v>
       </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A93">
+      <c r="E92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5">
+      <c r="A93" s="1">
+        <v>91</v>
+      </c>
+      <c r="B93">
         <v>8502</v>
       </c>
-      <c r="B93">
-        <v>0</v>
-      </c>
       <c r="C93">
         <v>0</v>
       </c>
       <c r="D93">
         <v>0</v>
       </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A94">
+      <c r="E93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5">
+      <c r="A94" s="1">
+        <v>92</v>
+      </c>
+      <c r="B94">
         <v>8549</v>
       </c>
-      <c r="B94">
-        <v>0</v>
-      </c>
       <c r="C94">
         <v>0</v>
       </c>
       <c r="D94">
         <v>0</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A95">
+      <c r="E94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5">
+      <c r="A95" s="1">
+        <v>93</v>
+      </c>
+      <c r="B95">
         <v>8537</v>
       </c>
-      <c r="B95">
-        <v>0</v>
-      </c>
       <c r="C95">
         <v>0</v>
       </c>
       <c r="D95">
         <v>0</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A96">
+      <c r="E95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5">
+      <c r="A96" s="1">
+        <v>94</v>
+      </c>
+      <c r="B96">
         <v>8506</v>
       </c>
-      <c r="B96">
-        <v>0</v>
-      </c>
       <c r="C96">
         <v>0</v>
       </c>
       <c r="D96">
         <v>0</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A97">
+      <c r="E96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5">
+      <c r="A97" s="1">
+        <v>95</v>
+      </c>
+      <c r="B97">
         <v>8492</v>
       </c>
-      <c r="B97">
-        <v>0</v>
-      </c>
       <c r="C97">
         <v>0</v>
       </c>
       <c r="D97">
         <v>0</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A98">
+      <c r="E97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5">
+      <c r="A98" s="1">
+        <v>96</v>
+      </c>
+      <c r="B98">
         <v>8503</v>
       </c>
-      <c r="B98">
-        <v>0</v>
-      </c>
       <c r="C98">
         <v>0</v>
       </c>
       <c r="D98">
         <v>0</v>
       </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A99">
+      <c r="E98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5">
+      <c r="A99" s="1">
+        <v>97</v>
+      </c>
+      <c r="B99">
         <v>8490</v>
       </c>
-      <c r="B99">
-        <v>0</v>
-      </c>
       <c r="C99">
         <v>0</v>
       </c>
       <c r="D99">
         <v>0</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A100">
+      <c r="E99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5">
+      <c r="A100" s="1">
+        <v>98</v>
+      </c>
+      <c r="B100">
         <v>8490</v>
       </c>
-      <c r="B100">
-        <v>0</v>
-      </c>
       <c r="C100">
         <v>0</v>
       </c>
       <c r="D100">
         <v>0</v>
       </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A101">
+      <c r="E100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5">
+      <c r="A101" s="1">
+        <v>99</v>
+      </c>
+      <c r="B101">
         <v>8524</v>
       </c>
-      <c r="B101">
-        <v>0</v>
-      </c>
       <c r="C101">
         <v>0</v>
       </c>
       <c r="D101">
         <v>0</v>
       </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A102">
+      <c r="E101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5">
+      <c r="A102" s="1">
+        <v>100</v>
+      </c>
+      <c r="B102">
         <v>8531</v>
       </c>
-      <c r="B102">
-        <v>0</v>
-      </c>
       <c r="C102">
         <v>0</v>
       </c>
       <c r="D102">
         <v>0</v>
       </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A103">
+      <c r="E102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5">
+      <c r="A103" s="1">
+        <v>101</v>
+      </c>
+      <c r="B103">
         <v>8534</v>
       </c>
-      <c r="B103">
-        <v>0</v>
-      </c>
       <c r="C103">
         <v>0</v>
       </c>
       <c r="D103">
         <v>0</v>
       </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A104">
+      <c r="E103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5">
+      <c r="A104" s="1">
+        <v>102</v>
+      </c>
+      <c r="B104">
         <v>8529</v>
       </c>
-      <c r="B104">
-        <v>0</v>
-      </c>
       <c r="C104">
         <v>0</v>
       </c>
       <c r="D104">
         <v>0</v>
       </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A105">
+      <c r="E104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5">
+      <c r="A105" s="1">
+        <v>103</v>
+      </c>
+      <c r="B105">
         <v>8538</v>
       </c>
-      <c r="B105">
-        <v>0</v>
-      </c>
       <c r="C105">
         <v>0</v>
       </c>
       <c r="D105">
         <v>0</v>
       </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A106">
+      <c r="E105">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5">
+      <c r="A106" s="1">
+        <v>104</v>
+      </c>
+      <c r="B106">
         <v>8522</v>
       </c>
-      <c r="B106">
-        <v>0</v>
-      </c>
       <c r="C106">
         <v>0</v>
       </c>
       <c r="D106">
         <v>0</v>
       </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A107">
+      <c r="E106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5">
+      <c r="A107" s="1">
+        <v>105</v>
+      </c>
+      <c r="B107">
         <v>8534</v>
       </c>
-      <c r="B107">
-        <v>0</v>
-      </c>
       <c r="C107">
         <v>0</v>
       </c>
       <c r="D107">
         <v>0</v>
       </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A108">
+      <c r="E107">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5">
+      <c r="A108" s="1">
+        <v>106</v>
+      </c>
+      <c r="B108">
         <v>8514</v>
       </c>
-      <c r="B108">
-        <v>0</v>
-      </c>
       <c r="C108">
         <v>0</v>
       </c>
       <c r="D108">
         <v>0</v>
       </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A109">
+      <c r="E108">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5">
+      <c r="A109" s="1">
+        <v>107</v>
+      </c>
+      <c r="B109">
         <v>8514</v>
       </c>
-      <c r="B109">
-        <v>0</v>
-      </c>
       <c r="C109">
         <v>0</v>
       </c>
       <c r="D109">
         <v>0</v>
       </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A110">
+      <c r="E109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5">
+      <c r="A110" s="1">
+        <v>108</v>
+      </c>
+      <c r="B110">
         <v>8503</v>
       </c>
-      <c r="B110">
-        <v>0</v>
-      </c>
       <c r="C110">
         <v>0</v>
       </c>
       <c r="D110">
         <v>0</v>
       </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A111">
+      <c r="E110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5">
+      <c r="A111" s="1">
+        <v>109</v>
+      </c>
+      <c r="B111">
         <v>8507</v>
       </c>
-      <c r="B111">
-        <v>0</v>
-      </c>
       <c r="C111">
         <v>0</v>
       </c>
       <c r="D111">
         <v>0</v>
       </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A112">
+      <c r="E111">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5">
+      <c r="A112" s="1">
+        <v>110</v>
+      </c>
+      <c r="B112">
         <v>8496</v>
       </c>
-      <c r="B112">
-        <v>0</v>
-      </c>
       <c r="C112">
         <v>0</v>
       </c>
       <c r="D112">
         <v>0</v>
       </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A113">
+      <c r="E112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5">
+      <c r="A113" s="1">
+        <v>111</v>
+      </c>
+      <c r="B113">
         <v>8507</v>
       </c>
-      <c r="B113">
-        <v>0</v>
-      </c>
       <c r="C113">
         <v>0</v>
       </c>
       <c r="D113">
         <v>0</v>
       </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A114">
+      <c r="E113">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5">
+      <c r="A114" s="1">
+        <v>112</v>
+      </c>
+      <c r="B114">
         <v>8498</v>
       </c>
-      <c r="B114">
-        <v>0</v>
-      </c>
       <c r="C114">
         <v>0</v>
       </c>
       <c r="D114">
         <v>0</v>
       </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A115">
+      <c r="E114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5">
+      <c r="A115" s="1">
+        <v>113</v>
+      </c>
+      <c r="B115">
         <v>8495</v>
       </c>
-      <c r="B115">
-        <v>0</v>
-      </c>
       <c r="C115">
         <v>0</v>
       </c>
       <c r="D115">
         <v>0</v>
       </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A116">
+      <c r="E115">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5">
+      <c r="A116" s="1">
+        <v>114</v>
+      </c>
+      <c r="B116">
         <v>8477</v>
       </c>
-      <c r="B116">
-        <v>0</v>
-      </c>
       <c r="C116">
         <v>0</v>
       </c>
       <c r="D116">
         <v>0</v>
       </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A117">
+      <c r="E116">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5">
+      <c r="A117" s="1">
+        <v>115</v>
+      </c>
+      <c r="B117">
         <v>8481</v>
       </c>
-      <c r="B117">
-        <v>0</v>
-      </c>
       <c r="C117">
         <v>0</v>
       </c>
       <c r="D117">
         <v>0</v>
       </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A118">
+      <c r="E117">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5">
+      <c r="A118" s="1">
+        <v>116</v>
+      </c>
+      <c r="B118">
         <v>8473</v>
       </c>
-      <c r="B118">
-        <v>0</v>
-      </c>
       <c r="C118">
         <v>0</v>
       </c>
       <c r="D118">
         <v>0</v>
       </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A119">
+      <c r="E118">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5">
+      <c r="A119" s="1">
+        <v>117</v>
+      </c>
+      <c r="B119">
         <v>8474</v>
       </c>
-      <c r="B119">
-        <v>0</v>
-      </c>
       <c r="C119">
         <v>0</v>
       </c>
       <c r="D119">
         <v>0</v>
       </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A120">
+      <c r="E119">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5">
+      <c r="A120" s="1">
+        <v>118</v>
+      </c>
+      <c r="B120">
         <v>8481</v>
       </c>
-      <c r="B120">
-        <v>0</v>
-      </c>
       <c r="C120">
         <v>0</v>
       </c>
       <c r="D120">
         <v>0</v>
       </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A121">
+      <c r="E120">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5">
+      <c r="A121" s="1">
+        <v>119</v>
+      </c>
+      <c r="B121">
         <v>8502</v>
       </c>
-      <c r="B121">
-        <v>0</v>
-      </c>
       <c r="C121">
         <v>0</v>
       </c>
       <c r="D121">
         <v>0</v>
       </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A122">
+      <c r="E121">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5">
+      <c r="A122" s="1">
+        <v>120</v>
+      </c>
+      <c r="B122">
         <v>8498</v>
       </c>
-      <c r="B122">
-        <v>0</v>
-      </c>
       <c r="C122">
         <v>0</v>
       </c>
       <c r="D122">
         <v>0</v>
       </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A123">
+      <c r="E122">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5">
+      <c r="A123" s="1">
+        <v>121</v>
+      </c>
+      <c r="B123">
         <v>8495</v>
       </c>
-      <c r="B123">
-        <v>0</v>
-      </c>
       <c r="C123">
         <v>0</v>
       </c>
       <c r="D123">
         <v>0</v>
       </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A124">
+      <c r="E123">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5">
+      <c r="A124" s="1">
+        <v>122</v>
+      </c>
+      <c r="B124">
         <v>8498</v>
       </c>
-      <c r="B124">
-        <v>0</v>
-      </c>
       <c r="C124">
         <v>0</v>
       </c>
       <c r="D124">
+        <v>0</v>
+      </c>
+      <c r="E124">
         <v>0</v>
       </c>
     </row>

</xml_diff>